<commit_message>
added round 3 data
</commit_message>
<xml_diff>
--- a/data/FinanceReport_r1.xlsx
+++ b/data/FinanceReport_r1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andris\Desktop\OP_Night_Shift\New_Dash\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EB5180-E55E-467E-AC8A-322D0FBE8D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B19504F-4EEE-4848-B462-F1F7C7A1CF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Output" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="75">
   <si>
     <t>ROI</t>
   </si>
@@ -240,6 +240,24 @@
   </si>
   <si>
     <t>Operating profit - Indirect cost - Project costs</t>
+  </si>
+  <si>
+    <t>Realized revenue - Contracted sales revenue - Contracted sales revenue - Webshop</t>
+  </si>
+  <si>
+    <t>Realized revenue - Cost of consumer returns</t>
+  </si>
+  <si>
+    <t>Realized revenue - Cost of consumer returns - Contracted sales revenue - Webshop</t>
+  </si>
+  <si>
+    <t>Gross margin - Cost of goods sold - Purchase value - Riesling</t>
+  </si>
+  <si>
+    <t>Gross margin - Cost of goods sold - Purchase value - Style cups</t>
+  </si>
+  <si>
+    <t>Gross margin - Cost of goods sold - Purchase value - BIG</t>
   </si>
 </sst>
 </file>
@@ -579,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +608,7 @@
     <col min="1" max="1" width="115.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -609,8 +627,11 @@
       <c r="F1" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,8 +650,11 @@
       <c r="F2" s="1">
         <v>3.7600000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <v>-0.4052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -649,8 +673,11 @@
       <c r="F3" s="1">
         <v>2025417.0722000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <v>2468418.6860000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -669,8 +696,11 @@
       <c r="F4" s="1">
         <v>323801.91480000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>620474.80630000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -689,1345 +719,1634 @@
       <c r="F5" s="1">
         <v>804786.2476</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>808896.29500000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>10413275.6973</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B7" s="1">
         <v>3127581.5441000001</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="1">
         <v>3127581.5441000001</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D7" s="1">
         <v>3127581.5441000001</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <v>3127581.5441000001</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>3154005.2346999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="G7" s="1">
+        <v>14311065.4847</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>-591938.74490000005</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="1">
         <v>-591938.74490000005</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>-591938.74490000005</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>-591938.74490000005</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>-90788.602899999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="G8" s="1">
+        <v>-568892.4192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
         <v>-80535.722200000004</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <v>-89660.946299999996</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>-89660.946299999996</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E9" s="1">
         <v>-89660.946299999996</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F9" s="1">
         <v>1616.769</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="G9" s="1">
+        <v>-23479.452700000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B10" s="1">
         <v>-40146.838900000002</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <v>-1036.347</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D10" s="1">
         <v>-1036.347</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>-1036.347</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>1209.0056</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="G10" s="1">
+        <v>76.125500000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B11" s="1">
         <v>-712621.30610000005</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <v>-682636.03830000001</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D11" s="1">
         <v>-682636.03830000001</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>-682636.03830000001</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>-87962.828200000004</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="G11" s="1">
+        <v>-592295.74639999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-3003829.5279999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <v>-3003829.5279999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B14" s="1">
         <v>2414960.2379999999</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C14" s="1">
         <v>2444945.5057999999</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D14" s="1">
         <v>2444945.5057999999</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E14" s="1">
         <v>2444945.5057999999</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F14" s="1">
         <v>3066042.4065</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="G14" s="1">
+        <v>10714940.210200001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <v>114432.3121</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="1">
         <v>124660.611</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D15" s="1">
         <v>124660.611</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E15" s="1">
         <v>124660.611</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F15" s="1">
         <v>116933.62420000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B16" s="1">
         <v>336595.10869999998</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C16" s="1">
         <v>350851.71120000002</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D16" s="1">
         <v>350851.71120000002</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E16" s="1">
         <v>350851.71120000002</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F16" s="1">
         <v>317913.07900000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="G16" s="1">
+        <v>317893.59169999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
+        <v>108158.04580000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B18" s="1">
         <v>550330.91769999999</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C18" s="1">
         <v>596592.00230000005</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D18" s="1">
         <v>596592.00230000005</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E18" s="1">
         <v>596592.00230000005</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F18" s="1">
         <v>542228.71010000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="G18" s="1">
+        <v>2615561.5304999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B19" s="1">
         <v>121346.1876</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C19" s="1">
         <v>127990.1211</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D19" s="1">
         <v>127990.1211</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E19" s="1">
         <v>127990.1211</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
         <v>108633.514</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="G20" s="1">
+        <v>109424.3125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1">
+        <v>2539688.9999000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B22" s="1">
         <v>8838.9976999999999</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C22" s="1">
         <v>8472.3274999999994</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D22" s="1">
         <v>8472.3274999999994</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E22" s="1">
         <v>8472.3274999999994</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F22" s="1">
         <v>8639.0226999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="G22" s="1">
+        <v>80462.4519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1">
+        <v>50149.654799999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B24" s="1">
         <v>9980.9650000000001</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C24" s="1">
         <v>9436.8045999999995</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D24" s="1">
         <v>9436.8045999999995</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E24" s="1">
         <v>9436.8045999999995</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
         <v>9353.2401000000009</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="G25" s="1">
+        <v>9021.8284999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B26" s="1">
         <v>1141524.4890999999</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C26" s="1">
         <v>1218003.5778999999</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D26" s="1">
         <v>1218003.5778999999</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E26" s="1">
         <v>1218003.5778999999</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F26" s="1">
         <v>1103701.1904</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="G26" s="1">
+        <v>5830360.4160000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B27" s="1">
         <v>50000</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C27" s="1">
         <v>50000</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D27" s="1">
         <v>50000</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E27" s="1">
         <v>50000</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F27" s="1">
         <v>50000</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="G27" s="1">
+        <v>92500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B28" s="1">
         <v>300000</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C28" s="1">
         <v>300000</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D28" s="1">
         <v>300000</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E28" s="1">
         <v>300000</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F28" s="1">
         <v>300000</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="G28" s="1">
+        <v>540000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B29" s="1">
         <v>10805.6468</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C29" s="1">
         <v>20218.564999999999</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D29" s="1">
         <v>20218.564999999999</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E29" s="1">
         <v>20218.564999999999</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F29" s="1">
         <v>1425.9945</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="G29" s="1">
+        <v>46138.318200000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
         <v>79.405299999999997</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D30" s="1">
         <v>79.405299999999997</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E30" s="1">
         <v>79.405299999999997</v>
       </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B31" s="1">
         <v>31250</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C31" s="1">
         <v>31250</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D31" s="1">
         <v>31250</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E31" s="1">
         <v>31250</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F31" s="1">
         <v>31250</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="G31" s="1">
+        <v>31250</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B32" s="1">
         <v>163533.41769999999</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C32" s="1">
         <v>173574.68350000001</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D32" s="1">
         <v>173574.68350000001</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E32" s="1">
         <v>173574.68350000001</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F32" s="1">
         <v>175811.01259999999</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="G32" s="1">
+        <v>282532.78480000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B33" s="1">
         <v>555589.06460000004</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C33" s="1">
         <v>575122.65390000003</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D33" s="1">
         <v>575122.65390000003</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E33" s="1">
         <v>575122.65390000003</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F33" s="1">
         <v>558487.00719999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="G33" s="1">
+        <v>992421.103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B34" s="1">
         <v>1697113.5537</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C34" s="1">
         <v>1793126.2319</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D34" s="1">
         <v>1793126.2319</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E34" s="1">
         <v>1793126.2319</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F34" s="1">
         <v>1662188.1976000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="G34" s="1">
+        <v>6822781.5190000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B35" s="1">
         <v>717846.68420000002</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C35" s="1">
         <v>651819.27390000003</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D35" s="1">
         <v>651819.27390000003</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E35" s="1">
         <v>651819.27390000003</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F35" s="1">
         <v>1403854.2087999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="G35" s="1">
+        <v>3892158.6910999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B36" s="1">
         <v>179558.99770000001</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C36" s="1">
         <v>192926.6281</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D36" s="1">
         <v>192926.6281</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E36" s="1">
         <v>192926.6281</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F36" s="1">
         <v>177818.55050000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="G36" s="1">
+        <v>296553.51179999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B37" s="1">
         <v>24638.207999999999</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C37" s="1">
         <v>24595.361700000001</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D37" s="1">
         <v>24595.361700000001</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E37" s="1">
         <v>24595.361700000001</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F37" s="1">
         <v>36544.851000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="G37" s="1">
+        <v>51505.059500000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B38" s="1">
         <v>162827.44630000001</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C38" s="1">
         <v>162827.44630000001</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D38" s="1">
         <v>162827.44630000001</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E38" s="1">
         <v>162827.44630000001</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F38" s="1">
         <v>163620.15700000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="G38" s="1">
+        <v>522581.9645</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B39" s="1">
         <v>367024.65210000001</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C39" s="1">
         <v>380349.4362</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D39" s="1">
         <v>380349.4362</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E39" s="1">
         <v>380349.4362</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F39" s="1">
         <v>377983.55849999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="G39" s="1">
+        <v>870640.53590000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B40" s="1">
         <v>11521.8431</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C40" s="1">
         <v>14700.744500000001</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D40" s="1">
         <v>14700.744500000001</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E40" s="1">
         <v>14700.744500000001</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F40" s="1">
         <v>13433.6795</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="G40" s="1">
+        <v>81618.602199999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B41" s="1">
         <v>11984.4696</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C41" s="1">
         <v>16838.488099999999</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D41" s="1">
         <v>16838.488099999999</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E41" s="1">
         <v>16838.488099999999</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F41" s="1">
         <v>15016.103300000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="G41" s="1">
+        <v>37381.464099999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B42" s="1">
         <v>23506.312699999999</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C42" s="1">
         <v>31539.2327</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D42" s="1">
         <v>31539.2327</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E42" s="1">
         <v>31539.2327</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F42" s="1">
         <v>28449.782899999998</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="G42" s="1">
+        <v>119000.06630000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B43" s="1">
         <v>100000</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C43" s="1">
         <v>100000</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D43" s="1">
         <v>100000</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E43" s="1">
         <v>100000</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F43" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="G43" s="1">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B44" s="1">
         <v>1296.1994999999999</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C44" s="1">
         <v>13402.6489</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D44" s="1">
         <v>13402.6489</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E44" s="1">
         <v>13402.6489</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F44" s="1">
         <v>5.8311999999999999</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="G44" s="1">
+        <v>58.2258</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B45" s="1">
         <v>28183.686600000001</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C45" s="1">
         <v>35445.380400000002</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D45" s="1">
         <v>35445.380400000002</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E45" s="1">
         <v>35445.380400000002</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F45" s="1">
         <v>38696.250800000002</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="G45" s="1">
+        <v>133669.06940000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B46" s="1">
         <v>120000</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C46" s="1">
         <v>120000</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D46" s="1">
         <v>120000</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E46" s="1">
         <v>120000</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F46" s="1">
         <v>120000</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="G46" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B47" s="1">
         <v>2887.9668999999999</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C47" s="1">
         <v>26725.661599999999</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D47" s="1">
         <v>26725.661599999999</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E47" s="1">
         <v>26725.661599999999</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F47" s="1">
         <v>10521.470600000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="G47" s="1">
+        <v>4943.8004000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B48" s="1">
         <v>252367.85310000001</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C48" s="1">
         <v>295573.6911</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D48" s="1">
         <v>295573.6911</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E48" s="1">
         <v>295573.6911</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F48" s="1">
         <v>269223.5527</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="G48" s="1">
+        <v>488671.09570000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B49" s="1">
         <v>31621.8269</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C49" s="1">
         <v>66445.333499999993</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D49" s="1">
         <v>66445.333499999993</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E49" s="1">
         <v>66445.333499999993</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F49" s="1">
         <v>28581.3812</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="G49" s="1">
+        <v>23589.148300000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B50" s="1">
         <v>31621.8269</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C50" s="1">
         <v>66445.333499999993</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D50" s="1">
         <v>66445.333499999993</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E50" s="1">
         <v>66445.333499999993</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F50" s="1">
         <v>28581.3812</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="G50" s="1">
+        <v>23589.148300000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B51" s="1">
         <v>307495.99280000001</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C51" s="1">
         <v>393558.2573</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D51" s="1">
         <v>393558.2573</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E51" s="1">
         <v>393558.2573</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F51" s="1">
         <v>326254.7169</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="G51" s="1">
+        <v>631260.31050000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B52" s="1">
         <v>60000</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C52" s="1">
         <v>60000</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D52" s="1">
         <v>60000</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E52" s="1">
         <v>60000</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F52" s="1">
         <v>60000</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="G52" s="1">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B53" s="1">
         <v>6771.0896000000002</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C53" s="1">
         <v>11123.6003</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D53" s="1">
         <v>11123.6003</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E53" s="1">
         <v>11123.6003</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F53" s="1">
         <v>3176.6282000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="G53" s="1">
+        <v>1970.2375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="1">
-        <v>0</v>
-      </c>
-      <c r="C48" s="1">
-        <v>0</v>
-      </c>
-      <c r="D48" s="1">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-      <c r="F48" s="1">
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
         <v>1101.5041000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="G54" s="1">
+        <v>2166.4539</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B55" s="1">
         <v>66771.089600000007</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C55" s="1">
         <v>71123.600300000006</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D55" s="1">
         <v>71123.600300000006</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E55" s="1">
         <v>71123.600300000006</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F55" s="1">
         <v>64278.132299999997</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="G55" s="1">
+        <v>84136.691399999996</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B56" s="1">
         <v>40000</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C56" s="1">
         <v>40000</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D56" s="1">
         <v>40000</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E56" s="1">
         <v>40000</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F56" s="1">
         <v>60000</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="G56" s="1">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B57" s="1">
         <v>45501.923000000003</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C57" s="1">
         <v>68598.060800000007</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D57" s="1">
         <v>68598.060800000007</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E57" s="1">
         <v>68598.060800000007</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F57" s="1">
         <v>19572.942899999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="G57" s="1">
+        <v>476311.79950000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B58" s="1">
         <v>85501.922999999995</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C58" s="1">
         <v>108598.06080000001</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D58" s="1">
         <v>108598.06080000001</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E58" s="1">
         <v>108598.06080000001</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F58" s="1">
         <v>79572.942899999995</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="G58" s="1">
+        <v>556311.79949999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B59" s="1">
         <v>152273.01269999999</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C59" s="1">
         <v>179721.6612</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D59" s="1">
         <v>179721.6612</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E59" s="1">
         <v>179721.6612</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F59" s="1">
         <v>143851.0753</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="G59" s="1">
+        <v>640448.49100000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B60" s="1">
         <v>291.27420000000001</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C60" s="1">
         <v>284.31150000000002</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D60" s="1">
         <v>284.31150000000002</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E60" s="1">
         <v>284.31150000000002</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F60" s="1">
         <v>450.54669999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="G60" s="1">
+        <v>525.68619999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B61" s="1">
         <v>1456.3713</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C61" s="1">
         <v>1421.5576000000001</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D61" s="1">
         <v>1421.5576000000001</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E61" s="1">
         <v>1421.5576000000001</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F61" s="1">
         <v>2252.7337000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="G61" s="1">
+        <v>2612.4748</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B62" s="1">
         <v>120000</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C62" s="1">
         <v>120000</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D62" s="1">
         <v>120000</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E62" s="1">
         <v>120000</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F62" s="1">
         <v>120000</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="G62" s="1">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B63" s="1">
         <v>121747.6456</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C63" s="1">
         <v>121705.8692</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D63" s="1">
         <v>121705.8692</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E63" s="1">
         <v>121705.8692</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F63" s="1">
         <v>122703.28049999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="G63" s="1">
+        <v>163138.1611</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B64" s="1">
         <v>888.85069999999996</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C64" s="1">
         <v>888.85069999999996</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D64" s="1">
         <v>888.85069999999996</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E64" s="1">
         <v>888.85069999999996</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F64" s="1">
         <v>889.02470000000005</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="G64" s="1">
+        <v>1209.9485999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B65" s="1">
         <v>7774.3248999999996</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C65" s="1">
         <v>7774.3248999999996</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D65" s="1">
         <v>7774.3248999999996</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E65" s="1">
         <v>7774.3248999999996</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F65" s="1">
         <v>7775.0501999999997</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="G65" s="1">
+        <v>466017.01689999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B66" s="1">
         <v>8663.1756000000005</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C66" s="1">
         <v>8663.1756000000005</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D66" s="1">
         <v>8663.1756000000005</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E66" s="1">
         <v>8663.1756000000005</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F66" s="1">
         <v>8664.0748999999996</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="G66" s="1">
+        <v>467226.9656</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B67" s="1">
         <v>130410.82120000001</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C67" s="1">
         <v>130369.0448</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D67" s="1">
         <v>130369.0448</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E67" s="1">
         <v>130369.0448</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F67" s="1">
         <v>131367.35550000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="G67" s="1">
+        <v>630365.12670000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B68" s="1">
         <v>216423.01939999999</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C68" s="1">
         <v>216423.01939999999</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D68" s="1">
         <v>216423.01939999999</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E68" s="1">
         <v>216423.01939999999</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F68" s="1">
         <v>216401.2028</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="G68" s="1">
+        <v>3496115.1033999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="1">
-        <v>0</v>
-      </c>
-      <c r="C63" s="1">
-        <v>0</v>
-      </c>
-      <c r="D63" s="1">
-        <v>0</v>
-      </c>
-      <c r="E63" s="1">
-        <v>0</v>
-      </c>
-      <c r="F63" s="1">
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
         <v>6000</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="G69" s="1">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="1">
-        <v>0</v>
-      </c>
-      <c r="C64" s="1">
-        <v>0</v>
-      </c>
-      <c r="D64" s="1">
-        <v>0</v>
-      </c>
-      <c r="E64" s="1">
-        <v>0</v>
-      </c>
-      <c r="F64" s="1">
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0</v>
+      </c>
+      <c r="F70" s="1">
         <v>15000</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="G70" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="1">
-        <v>0</v>
-      </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="1">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1">
-        <v>0</v>
-      </c>
-      <c r="F65" s="1">
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1">
         <v>21000</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="G71" s="1">
+        <v>40800</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B72" s="1">
         <v>20837.6119</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C72" s="1">
         <v>21354.099300000002</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D72" s="1">
         <v>21354.099300000002</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E72" s="1">
         <v>21354.099300000002</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F72" s="1">
         <v>32023.6842</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="G72" s="1">
+        <v>58951.532399999996</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B73" s="1">
         <v>1194465.1102</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C73" s="1">
         <v>1321775.5183999999</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D73" s="1">
         <v>1321775.5183999999</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E73" s="1">
         <v>1321775.5183999999</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F73" s="1">
         <v>1248881.5935</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="G73" s="1">
+        <v>6368581.1001000004</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B74" s="1">
         <v>-476618.42589999997</v>
       </c>
-      <c r="C68" s="1">
+      <c r="C74" s="1">
         <v>-669956.24450000003</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D74" s="1">
         <v>-669956.24450000003</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E74" s="1">
         <v>-669956.24450000003</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F74" s="1">
         <v>154972.6153</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="G74" s="1">
+        <v>-2476422.4089000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B75" s="1">
         <v>2500000</v>
       </c>
-      <c r="C69" s="1">
+      <c r="C75" s="1">
         <v>2500000</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D75" s="1">
         <v>2500000</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E75" s="1">
         <v>2500000</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F75" s="1">
         <v>2500000</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="G75" s="1">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B76" s="1">
         <v>313417.50290000002</v>
       </c>
-      <c r="C70" s="1">
+      <c r="C76" s="1">
         <v>420523.1029</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D76" s="1">
         <v>420523.1029</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E76" s="1">
         <v>420523.1029</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F76" s="1">
         <v>379330.43930000003</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="G76" s="1">
+        <v>1586667.5518</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B77" s="1">
         <v>812500</v>
       </c>
-      <c r="C71" s="1">
+      <c r="C77" s="1">
         <v>812500</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D77" s="1">
         <v>812500</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E77" s="1">
         <v>812500</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F77" s="1">
         <v>812500</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="G77" s="1">
+        <v>1237500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B78" s="1">
         <v>277834.82559999998</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C78" s="1">
         <v>284721.32419999997</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D78" s="1">
         <v>284721.32419999997</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E78" s="1">
         <v>284721.32419999997</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F78" s="1">
         <v>426982.45699999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="G78" s="1">
+        <v>786020.43240000005</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B79" s="1">
         <v>3903752.3284999998</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C79" s="1">
         <v>4017744.4271999998</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D79" s="1">
         <v>4017744.4271999998</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E79" s="1">
         <v>4017744.4271999998</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F79" s="1">
         <v>4118812.8963000001</v>
+      </c>
+      <c r="G79" s="1">
+        <v>6110187.9841999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>